<commit_message>
Updating Burn Down Chart
</commit_message>
<xml_diff>
--- a/Sprint4BurndownChart.xlsx
+++ b/Sprint4BurndownChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\OneDrive\Desktop\Trophyyyy\Trophy-Hoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph Earl\Desktop\New folder\Trophy-Hoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD09EAF8-3E1D-48CE-A812-8EC591290D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A502B7-BC3E-4BA4-91A6-62304D7D8B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{880ECEA2-B438-484A-9CBA-91374F2777E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{880ECEA2-B438-484A-9CBA-91374F2777E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Iteration" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Product Backlog Items</t>
-  </si>
-  <si>
-    <t>Feature 2</t>
   </si>
   <si>
     <t>Feature 3</t>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Austin - Add Trail and Finishing Touches to Fireball</t>
+  </si>
+  <si>
+    <t>Cleaning Existing Modes &amp; Dungeon Level Creation</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1058,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -1251,67 +1251,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.2</c:v>
+                  <c:v>53.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.399999999999999</c:v>
+                  <c:v>50.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.599999999999998</c:v>
+                  <c:v>47.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.799999999999997</c:v>
+                  <c:v>44.800000000000011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.999999999999996</c:v>
+                  <c:v>42.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.199999999999996</c:v>
+                  <c:v>39.200000000000017</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.399999999999995</c:v>
+                  <c:v>36.40000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.5999999999999943</c:v>
+                  <c:v>33.600000000000023</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.7999999999999936</c:v>
+                  <c:v>30.800000000000022</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.9999999999999938</c:v>
+                  <c:v>28.000000000000021</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.199999999999994</c:v>
+                  <c:v>25.200000000000021</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.3999999999999941</c:v>
+                  <c:v>22.40000000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.5999999999999943</c:v>
+                  <c:v>19.600000000000019</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.7999999999999945</c:v>
+                  <c:v>16.800000000000018</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.9999999999999947</c:v>
+                  <c:v>14.000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.1999999999999948</c:v>
+                  <c:v>11.200000000000017</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.399999999999995</c:v>
+                  <c:v>8.4000000000000163</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.599999999999995</c:v>
+                  <c:v>5.6000000000000165</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.79999999999999494</c:v>
+                  <c:v>2.8000000000000167</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-5.1070259132757201E-15</c:v>
+                  <c:v>1.6875389974302379E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1788,7 +1788,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -2030,67 +2030,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.2</c:v>
+                  <c:v>53.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.399999999999999</c:v>
+                  <c:v>50.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.599999999999998</c:v>
+                  <c:v>47.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.799999999999997</c:v>
+                  <c:v>44.800000000000011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.999999999999996</c:v>
+                  <c:v>42.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.199999999999996</c:v>
+                  <c:v>39.200000000000017</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.399999999999995</c:v>
+                  <c:v>36.40000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.5999999999999943</c:v>
+                  <c:v>33.600000000000023</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.7999999999999936</c:v>
+                  <c:v>30.800000000000022</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.9999999999999938</c:v>
+                  <c:v>28.000000000000021</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.199999999999994</c:v>
+                  <c:v>25.200000000000021</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.3999999999999941</c:v>
+                  <c:v>22.40000000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.5999999999999943</c:v>
+                  <c:v>19.600000000000019</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.7999999999999945</c:v>
+                  <c:v>16.800000000000018</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.9999999999999947</c:v>
+                  <c:v>14.000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.1999999999999948</c:v>
+                  <c:v>11.200000000000017</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.399999999999995</c:v>
+                  <c:v>8.4000000000000163</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.599999999999995</c:v>
+                  <c:v>5.6000000000000165</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.79999999999999494</c:v>
+                  <c:v>2.8000000000000167</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-5.1070259132757201E-15</c:v>
+                  <c:v>1.6875389974302379E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3905,18 +3905,18 @@
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="22" width="5.7109375" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="22" width="5.6640625" customWidth="1"/>
+    <col min="24" max="24" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="37"/>
       <c r="B1" s="37"/>
       <c r="C1" s="6"/>
@@ -3942,11 +3942,11 @@
       <c r="W1" s="15"/>
       <c r="X1" s="16"/>
     </row>
-    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="40"/>
       <c r="E2" s="40"/>
@@ -3970,18 +3970,18 @@
       <c r="W2" s="15"/>
       <c r="X2" s="16"/>
     </row>
-    <row r="3" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="40"/>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
       <c r="G3" s="33">
         <f>B38</f>
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="H3" s="43"/>
       <c r="I3" s="43"/>
@@ -4001,11 +4001,11 @@
       <c r="W3" s="15"/>
       <c r="X3" s="16"/>
     </row>
-    <row r="4" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="40"/>
       <c r="E4" s="40"/>
@@ -4029,7 +4029,7 @@
       <c r="W4" s="15"/>
       <c r="X4" s="16"/>
     </row>
-    <row r="5" spans="1:24" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="97.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="34" t="s">
         <v>0</v>
       </c>
@@ -4057,13 +4057,13 @@
       <c r="W5" s="15"/>
       <c r="X5" s="16"/>
     </row>
-    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="39" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
@@ -4085,16 +4085,16 @@
       <c r="U6" s="38"/>
       <c r="V6" s="38"/>
       <c r="W6" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X6" s="42"/>
     </row>
-    <row r="7" spans="1:24" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -4157,15 +4157,15 @@
         <v>20</v>
       </c>
       <c r="W7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="X7" s="9" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="8" spans="1:24" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="18">
         <v>16</v>
@@ -4199,11 +4199,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="21"/>
+        <v>42</v>
+      </c>
+      <c r="B9" s="21">
+        <v>40</v>
+      </c>
       <c r="C9" s="22"/>
       <c r="D9" s="23"/>
       <c r="E9" s="22"/>
@@ -4226,16 +4228,16 @@
       <c r="V9" s="23"/>
       <c r="W9" s="28">
         <f t="shared" ref="W9:W37" si="0">B9-SUM(C9:V9)</f>
+        <v>40</v>
+      </c>
+      <c r="X9" s="17">
+        <f>IFERROR(1-(W9/B9),"")</f>
         <v>0</v>
       </c>
-      <c r="X9" s="17" t="str">
-        <f>IFERROR(1-(W9/B9),"")</f>
-        <v/>
-      </c>
     </row>
-    <row r="10" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="22"/>
@@ -4267,9 +4269,9 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
@@ -4301,9 +4303,9 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
@@ -4335,9 +4337,9 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
@@ -4369,9 +4371,9 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
@@ -4403,9 +4405,9 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
@@ -4437,9 +4439,9 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="22"/>
@@ -4471,9 +4473,9 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="22"/>
@@ -4505,9 +4507,9 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
@@ -4539,9 +4541,9 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
@@ -4573,9 +4575,9 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
@@ -4607,9 +4609,9 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
@@ -4641,9 +4643,9 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
@@ -4675,9 +4677,9 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
@@ -4709,9 +4711,9 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
@@ -4743,9 +4745,9 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
@@ -4777,9 +4779,9 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
@@ -4811,9 +4813,9 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
@@ -4845,9 +4847,9 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
@@ -4879,9 +4881,9 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
@@ -4913,9 +4915,9 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="22"/>
@@ -4947,9 +4949,9 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="22"/>
@@ -4981,9 +4983,9 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
@@ -5015,9 +5017,9 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="22"/>
@@ -5049,9 +5051,9 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="22"/>
@@ -5083,9 +5085,9 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="22"/>
@@ -5117,9 +5119,9 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="22"/>
@@ -5151,9 +5153,9 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" s="24"/>
       <c r="C37" s="25"/>
@@ -5185,13 +5187,13 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A38" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="10">
         <f>SUM(B8:B37)</f>
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C38" s="11" t="e">
         <f>IFERROR(IF(B38-SUM(C8:C37)=B38,NA(),B38-SUM(C8:C37)),NA())</f>
@@ -5275,105 +5277,105 @@
       </c>
       <c r="W38" s="35">
         <f>SUM(W8:W37)</f>
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="X38" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="12">
         <f>SUM(B8:B37)</f>
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C39" s="13">
         <f>IFERROR((IF(B39-($B$38/$G$4) &lt; 0,"-", B39-($B$38/$G$4))),IFERROR(B39-($B$38/20),"-"))</f>
-        <v>15.2</v>
+        <v>53.2</v>
       </c>
       <c r="D39" s="13">
         <f t="shared" ref="D39:V39" si="3">IFERROR((IF(C39-($B$38/$G$4) &lt; 0,"-", C39-($B$38/$G$4))),IFERROR(C39-($B$38/20),"-"))</f>
-        <v>14.399999999999999</v>
+        <v>50.400000000000006</v>
       </c>
       <c r="E39" s="13">
         <f t="shared" si="3"/>
-        <v>13.599999999999998</v>
+        <v>47.600000000000009</v>
       </c>
       <c r="F39" s="13">
         <f t="shared" si="3"/>
-        <v>12.799999999999997</v>
+        <v>44.800000000000011</v>
       </c>
       <c r="G39" s="13">
         <f t="shared" si="3"/>
-        <v>11.999999999999996</v>
+        <v>42.000000000000014</v>
       </c>
       <c r="H39" s="13">
         <f t="shared" si="3"/>
-        <v>11.199999999999996</v>
+        <v>39.200000000000017</v>
       </c>
       <c r="I39" s="13">
         <f t="shared" si="3"/>
-        <v>10.399999999999995</v>
+        <v>36.40000000000002</v>
       </c>
       <c r="J39" s="13">
         <f t="shared" si="3"/>
-        <v>9.5999999999999943</v>
+        <v>33.600000000000023</v>
       </c>
       <c r="K39" s="13">
         <f t="shared" si="3"/>
-        <v>8.7999999999999936</v>
+        <v>30.800000000000022</v>
       </c>
       <c r="L39" s="13">
         <f t="shared" si="3"/>
-        <v>7.9999999999999938</v>
+        <v>28.000000000000021</v>
       </c>
       <c r="M39" s="13">
         <f t="shared" si="3"/>
-        <v>7.199999999999994</v>
+        <v>25.200000000000021</v>
       </c>
       <c r="N39" s="13">
         <f t="shared" si="3"/>
-        <v>6.3999999999999941</v>
+        <v>22.40000000000002</v>
       </c>
       <c r="O39" s="13">
         <f t="shared" si="3"/>
-        <v>5.5999999999999943</v>
+        <v>19.600000000000019</v>
       </c>
       <c r="P39" s="13">
         <f t="shared" si="3"/>
-        <v>4.7999999999999945</v>
+        <v>16.800000000000018</v>
       </c>
       <c r="Q39" s="13">
         <f t="shared" si="3"/>
-        <v>3.9999999999999947</v>
+        <v>14.000000000000018</v>
       </c>
       <c r="R39" s="13">
         <f t="shared" si="3"/>
-        <v>3.1999999999999948</v>
+        <v>11.200000000000017</v>
       </c>
       <c r="S39" s="13">
         <f t="shared" si="3"/>
-        <v>2.399999999999995</v>
+        <v>8.4000000000000163</v>
       </c>
       <c r="T39" s="13">
         <f t="shared" si="3"/>
-        <v>1.599999999999995</v>
+        <v>5.6000000000000165</v>
       </c>
       <c r="U39" s="13">
         <f t="shared" si="3"/>
-        <v>0.79999999999999494</v>
+        <v>2.8000000000000167</v>
       </c>
       <c r="V39" s="13">
         <f t="shared" si="3"/>
-        <v>-5.1070259132757201E-15</v>
+        <v>1.6875389974302379E-14</v>
       </c>
       <c r="W39" s="31"/>
       <c r="X39" s="32"/>
     </row>
-    <row r="40" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:24" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A1:B2"/>
@@ -5437,7 +5439,7 @@
       <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>